<commit_message>
Fixed Subj_ID to be unique
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Stevia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC286F01-82F1-4DBB-B5A7-1C31073ADA16}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628175A1-9BED-4434-B2E0-25FC50F41ABE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{DE68B47F-C64E-46B0-840B-CBBCFE996E82}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="139">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -50,90 +50,60 @@
     <t>FL10A</t>
   </si>
   <si>
-    <t>SUBJ10</t>
-  </si>
-  <si>
     <t>FL10C</t>
   </si>
   <si>
     <t>FL1A</t>
   </si>
   <si>
-    <t>SUBJ1</t>
-  </si>
-  <si>
     <t>FL1C</t>
   </si>
   <si>
     <t>FL2A</t>
   </si>
   <si>
-    <t>SUBJ2</t>
-  </si>
-  <si>
     <t>FL2C</t>
   </si>
   <si>
     <t>FL3A</t>
   </si>
   <si>
-    <t>SUBJ3</t>
-  </si>
-  <si>
     <t>FL3C</t>
   </si>
   <si>
     <t>FL4A</t>
   </si>
   <si>
-    <t>SUBJ4</t>
-  </si>
-  <si>
     <t>FL4C</t>
   </si>
   <si>
     <t>FL5A</t>
   </si>
   <si>
-    <t>SUBJ5</t>
-  </si>
-  <si>
     <t>FL5C</t>
   </si>
   <si>
     <t>FL6A</t>
   </si>
   <si>
-    <t>SUBJ6</t>
-  </si>
-  <si>
     <t>FL6C</t>
   </si>
   <si>
     <t>FL7A</t>
   </si>
   <si>
-    <t>SUBJ7</t>
-  </si>
-  <si>
     <t>FL7C</t>
   </si>
   <si>
     <t>FL8A</t>
   </si>
   <si>
-    <t>SUBJ8</t>
-  </si>
-  <si>
     <t>FL8C</t>
   </si>
   <si>
     <t>FL9A</t>
   </si>
   <si>
-    <t>SUBJ9</t>
-  </si>
-  <si>
     <t>FL9C</t>
   </si>
   <si>
@@ -357,6 +327,126 @@
   </si>
   <si>
     <t>TV8A</t>
+  </si>
+  <si>
+    <t>FL1</t>
+  </si>
+  <si>
+    <t>FL2</t>
+  </si>
+  <si>
+    <t>FL3</t>
+  </si>
+  <si>
+    <t>FL4</t>
+  </si>
+  <si>
+    <t>FL5</t>
+  </si>
+  <si>
+    <t>FL6</t>
+  </si>
+  <si>
+    <t>FL7</t>
+  </si>
+  <si>
+    <t>FL8</t>
+  </si>
+  <si>
+    <t>FL9</t>
+  </si>
+  <si>
+    <t>FL10</t>
+  </si>
+  <si>
+    <t>HF1</t>
+  </si>
+  <si>
+    <t>HF2</t>
+  </si>
+  <si>
+    <t>HF3</t>
+  </si>
+  <si>
+    <t>HF4</t>
+  </si>
+  <si>
+    <t>HF5</t>
+  </si>
+  <si>
+    <t>HF6</t>
+  </si>
+  <si>
+    <t>HF7</t>
+  </si>
+  <si>
+    <t>HF8</t>
+  </si>
+  <si>
+    <t>HF9</t>
+  </si>
+  <si>
+    <t>HF10</t>
+  </si>
+  <si>
+    <t>SC1</t>
+  </si>
+  <si>
+    <t>SC2</t>
+  </si>
+  <si>
+    <t>SC3</t>
+  </si>
+  <si>
+    <t>SC4</t>
+  </si>
+  <si>
+    <t>SC5</t>
+  </si>
+  <si>
+    <t>SC6</t>
+  </si>
+  <si>
+    <t>SC7</t>
+  </si>
+  <si>
+    <t>SC8</t>
+  </si>
+  <si>
+    <t>SC9</t>
+  </si>
+  <si>
+    <t>SC10</t>
+  </si>
+  <si>
+    <t>TV1</t>
+  </si>
+  <si>
+    <t>TV2</t>
+  </si>
+  <si>
+    <t>TV3</t>
+  </si>
+  <si>
+    <t>TV4</t>
+  </si>
+  <si>
+    <t>TV5</t>
+  </si>
+  <si>
+    <t>TV6</t>
+  </si>
+  <si>
+    <t>TV7</t>
+  </si>
+  <si>
+    <t>TV8</t>
+  </si>
+  <si>
+    <t>TV9</t>
+  </si>
+  <si>
+    <t>TV10</t>
   </si>
 </sst>
 </file>
@@ -720,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F580D838-176B-498F-A508-C3968484E9F8}">
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,367 +836,367 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>101</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>101</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>105</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>105</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1114,1159 +1204,1159 @@
         <v>5</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>18</v>
+        <v>112</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>18</v>
+        <v>112</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>24</v>
+        <v>114</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>24</v>
+        <v>114</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>30</v>
+        <v>116</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D39" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>9</v>
+        <v>119</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>9</v>
+        <v>119</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>18</v>
+        <v>122</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>21</v>
+        <v>123</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>21</v>
+        <v>123</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>24</v>
+        <v>124</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E50" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>24</v>
+        <v>124</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>27</v>
+        <v>125</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E52" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>27</v>
+        <v>125</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>30</v>
+        <v>126</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E54" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>30</v>
+        <v>126</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>33</v>
+        <v>127</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E56" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>33</v>
+        <v>127</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>6</v>
+        <v>128</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E58" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>6</v>
+        <v>128</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>9</v>
+        <v>129</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>9</v>
+        <v>129</v>
       </c>
       <c r="C61" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>12</v>
+        <v>130</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>15</v>
+        <v>131</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>15</v>
+        <v>131</v>
       </c>
       <c r="C64" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F64" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>18</v>
+        <v>132</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>18</v>
+        <v>132</v>
       </c>
       <c r="C66" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F66" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>21</v>
+        <v>133</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>21</v>
+        <v>133</v>
       </c>
       <c r="C68" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F68" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>24</v>
+        <v>134</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>24</v>
+        <v>134</v>
       </c>
       <c r="C70" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F70" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>27</v>
+        <v>135</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C72" s="2" t="s">
+      <c r="D72" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F72" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>30</v>
+        <v>136</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>33</v>
+        <v>137</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>33</v>
+        <v>137</v>
       </c>
       <c r="C75" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F75" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>6</v>
+        <v>138</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>6</v>
+        <v>138</v>
       </c>
       <c r="C77" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added body weight & blood glucose
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Stevia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628175A1-9BED-4434-B2E0-25FC50F41ABE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6C119C-3D40-446E-8886-4E144CE742B1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{DE68B47F-C64E-46B0-840B-CBBCFE996E82}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="142">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -447,6 +447,15 @@
   </si>
   <si>
     <t>TV10</t>
+  </si>
+  <si>
+    <t>Body_Weight</t>
+  </si>
+  <si>
+    <t>Blood_Glucose</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -808,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F580D838-176B-498F-A508-C3968484E9F8}">
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -819,7 +828,7 @@
     <col min="1" max="5" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -838,8 +847,14 @@
       <c r="F1" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -858,8 +873,14 @@
       <c r="F2" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>22</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -878,8 +899,14 @@
       <c r="F3" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>26.9</v>
+      </c>
+      <c r="H3">
+        <v>21785</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -898,8 +925,14 @@
       <c r="F4" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>20.8</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -918,8 +951,14 @@
       <c r="F5" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>24.7</v>
+      </c>
+      <c r="H5">
+        <v>25870</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -938,8 +977,14 @@
       <c r="F6" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>18</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -958,8 +1003,14 @@
       <c r="F7" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>23.6</v>
+      </c>
+      <c r="H7">
+        <v>22330</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -978,8 +1029,14 @@
       <c r="F8" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>18</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -998,8 +1055,14 @@
       <c r="F9" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>23</v>
+      </c>
+      <c r="H9">
+        <v>19890</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1018,8 +1081,14 @@
       <c r="F10" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>25.8</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1038,8 +1107,14 @@
       <c r="F11" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>27.9</v>
+      </c>
+      <c r="H11">
+        <v>17870</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1058,8 +1133,14 @@
       <c r="F12" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>17.3</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1078,8 +1159,14 @@
       <c r="F13" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13" s="2">
+        <v>21.5</v>
+      </c>
+      <c r="H13">
+        <v>22890</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1098,8 +1185,14 @@
       <c r="F14" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <v>24.6</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -1118,8 +1211,14 @@
       <c r="F15" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <v>30</v>
+      </c>
+      <c r="H15">
+        <v>35875</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -1138,8 +1237,14 @@
       <c r="F16" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1158,8 +1263,14 @@
       <c r="F17" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <v>20</v>
+      </c>
+      <c r="H17">
+        <v>21607.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1178,8 +1289,14 @@
       <c r="F18" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>22.1</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -1198,8 +1315,14 @@
       <c r="F19" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>26.6</v>
+      </c>
+      <c r="H19">
+        <v>26352.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>5</v>
       </c>
@@ -1218,8 +1341,14 @@
       <c r="F20" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <v>25.6</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>6</v>
       </c>
@@ -1238,8 +1367,14 @@
       <c r="F21" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21">
+        <v>30.6</v>
+      </c>
+      <c r="H21">
+        <v>22760</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
@@ -1258,8 +1393,14 @@
       <c r="F22" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <v>24.1</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
@@ -1278,8 +1419,14 @@
       <c r="F23" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <v>51.3</v>
+      </c>
+      <c r="H23">
+        <v>54187.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
@@ -1298,8 +1445,14 @@
       <c r="F24" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <v>17.5</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
@@ -1318,8 +1471,14 @@
       <c r="F25" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <v>34.6</v>
+      </c>
+      <c r="H25">
+        <v>40387.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
@@ -1338,8 +1497,14 @@
       <c r="F26" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26">
+        <v>23.2</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
@@ -1358,8 +1523,14 @@
       <c r="F27" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <v>46.6</v>
+      </c>
+      <c r="H27">
+        <v>38932.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
@@ -1378,8 +1549,14 @@
       <c r="F28" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <v>24.8</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
@@ -1398,8 +1575,14 @@
       <c r="F29" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29">
+        <v>49.9</v>
+      </c>
+      <c r="H29">
+        <v>57077.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>35</v>
       </c>
@@ -1418,8 +1601,14 @@
       <c r="F30" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
@@ -1438,8 +1627,14 @@
       <c r="F31" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31">
+        <v>46.5</v>
+      </c>
+      <c r="H31">
+        <v>37397.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>37</v>
       </c>
@@ -1458,8 +1653,14 @@
       <c r="F32" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>38</v>
       </c>
@@ -1478,8 +1679,14 @@
       <c r="F33" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="H33">
+        <v>37837.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
@@ -1498,8 +1705,14 @@
       <c r="F34" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>40</v>
       </c>
@@ -1518,8 +1731,14 @@
       <c r="F35" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35">
+        <v>27.7</v>
+      </c>
+      <c r="H35">
+        <v>28442.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
@@ -1538,8 +1757,14 @@
       <c r="F36" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36">
+        <v>42.1</v>
+      </c>
+      <c r="H36" s="2">
+        <v>36430</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>42</v>
       </c>
@@ -1558,8 +1783,14 @@
       <c r="F37" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37">
+        <v>23.8</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
@@ -1578,8 +1809,14 @@
       <c r="F38" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38">
+        <v>53.4</v>
+      </c>
+      <c r="H38" s="2">
+        <v>56740</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>25</v>
       </c>
@@ -1598,8 +1835,14 @@
       <c r="F39" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39">
+        <v>23.8</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>26</v>
       </c>
@@ -1618,8 +1861,14 @@
       <c r="F40" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40">
+        <v>48.7</v>
+      </c>
+      <c r="H40" s="2">
+        <v>29777.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>46</v>
       </c>
@@ -1638,8 +1887,14 @@
       <c r="F41" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G41">
+        <v>26</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>47</v>
       </c>
@@ -1658,8 +1913,14 @@
       <c r="F42" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G42">
+        <v>47.7</v>
+      </c>
+      <c r="H42">
+        <v>45385</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>48</v>
       </c>
@@ -1678,8 +1939,14 @@
       <c r="F43" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G43">
+        <v>23</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>49</v>
       </c>
@@ -1698,8 +1965,14 @@
       <c r="F44" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G44">
+        <v>48.4</v>
+      </c>
+      <c r="H44">
+        <v>39175</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>50</v>
       </c>
@@ -1718,8 +1991,14 @@
       <c r="F45" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G45">
+        <v>25</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
@@ -1738,8 +2017,14 @@
       <c r="F46" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G46">
+        <v>48.1</v>
+      </c>
+      <c r="H46">
+        <v>48645.833299999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>52</v>
       </c>
@@ -1758,8 +2043,14 @@
       <c r="F47" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G47">
+        <v>22.2</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>53</v>
       </c>
@@ -1778,8 +2069,14 @@
       <c r="F48" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G48">
+        <v>25.8</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>54</v>
       </c>
@@ -1798,8 +2095,14 @@
       <c r="F49" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49">
+        <v>49.8</v>
+      </c>
+      <c r="H49">
+        <v>48600</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>55</v>
       </c>
@@ -1818,8 +2121,14 @@
       <c r="F50" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G50">
+        <v>18.3</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>56</v>
       </c>
@@ -1838,8 +2147,11 @@
       <c r="F51" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G51">
+        <v>48.4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>57</v>
       </c>
@@ -1858,8 +2170,14 @@
       <c r="F52" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G52">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>58</v>
       </c>
@@ -1878,8 +2196,14 @@
       <c r="F53" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G53">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="H53">
+        <v>32765</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
@@ -1898,8 +2222,14 @@
       <c r="F54" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G54">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>60</v>
       </c>
@@ -1918,8 +2248,14 @@
       <c r="F55" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G55">
+        <v>31.1</v>
+      </c>
+      <c r="H55">
+        <v>32342.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>61</v>
       </c>
@@ -1938,8 +2274,14 @@
       <c r="F56" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G56">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>62</v>
       </c>
@@ -1958,8 +2300,14 @@
       <c r="F57" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G57">
+        <v>38.1</v>
+      </c>
+      <c r="H57">
+        <v>24667.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>44</v>
       </c>
@@ -1978,8 +2326,14 @@
       <c r="F58" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G58">
+        <v>20</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>45</v>
       </c>
@@ -1998,8 +2352,14 @@
       <c r="F59" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G59">
+        <v>37</v>
+      </c>
+      <c r="H59">
+        <v>29167.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>65</v>
       </c>
@@ -2018,8 +2378,14 @@
       <c r="F60" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G60">
+        <v>22.2</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>66</v>
       </c>
@@ -2038,8 +2404,14 @@
       <c r="F61" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G61">
+        <v>47.8</v>
+      </c>
+      <c r="H61">
+        <v>39510</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>67</v>
       </c>
@@ -2058,8 +2430,14 @@
       <c r="F62" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G62">
+        <v>24</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>68</v>
       </c>
@@ -2078,8 +2456,14 @@
       <c r="F63" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G63">
+        <v>23.5</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>69</v>
       </c>
@@ -2098,8 +2482,14 @@
       <c r="F64" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G64">
+        <v>50.3</v>
+      </c>
+      <c r="H64" s="2">
+        <v>47517.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>70</v>
       </c>
@@ -2118,8 +2508,14 @@
       <c r="F65" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G65">
+        <v>25.9</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>71</v>
       </c>
@@ -2138,8 +2534,14 @@
       <c r="F66" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G66">
+        <v>49.1</v>
+      </c>
+      <c r="H66">
+        <v>58777.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>72</v>
       </c>
@@ -2158,8 +2560,14 @@
       <c r="F67" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G67">
+        <v>17.3</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>73</v>
       </c>
@@ -2178,8 +2586,14 @@
       <c r="F68" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G68">
+        <v>27.4</v>
+      </c>
+      <c r="H68">
+        <v>30347.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>74</v>
       </c>
@@ -2198,8 +2612,14 @@
       <c r="F69" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G69">
+        <v>18.5</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>75</v>
       </c>
@@ -2218,8 +2638,14 @@
       <c r="F70" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G70">
+        <v>43.4</v>
+      </c>
+      <c r="H70">
+        <v>39465</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>76</v>
       </c>
@@ -2238,8 +2664,14 @@
       <c r="F71" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G71">
+        <v>25.4</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>77</v>
       </c>
@@ -2258,8 +2690,14 @@
       <c r="F72" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G72">
+        <v>49.8</v>
+      </c>
+      <c r="H72">
+        <v>50897.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>98</v>
       </c>
@@ -2278,8 +2716,14 @@
       <c r="F73" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G73">
+        <v>19.7</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>78</v>
       </c>
@@ -2298,8 +2742,14 @@
       <c r="F74" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G74">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>79</v>
       </c>
@@ -2318,8 +2768,14 @@
       <c r="F75" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G75">
+        <v>46.4</v>
+      </c>
+      <c r="H75">
+        <v>35699.166669999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>63</v>
       </c>
@@ -2338,8 +2794,14 @@
       <c r="F76" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G76">
+        <v>17</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>64</v>
       </c>
@@ -2357,6 +2819,12 @@
       </c>
       <c r="F77" s="2" t="s">
         <v>97</v>
+      </c>
+      <c r="G77">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="H77">
+        <v>27257.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated metadata with correct body weights
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Stevia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6C119C-3D40-446E-8886-4E144CE742B1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EE241D-93BC-4E71-9028-A842EE49667C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{DE68B47F-C64E-46B0-840B-CBBCFE996E82}"/>
   </bookViews>
@@ -819,7 +819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F580D838-176B-498F-A508-C3968484E9F8}">
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
       <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
@@ -874,7 +874,7 @@
         <v>89</v>
       </c>
       <c r="G2">
-        <v>22</v>
+        <v>23.2</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>141</v>
@@ -900,7 +900,7 @@
         <v>90</v>
       </c>
       <c r="G3">
-        <v>26.9</v>
+        <v>26.7</v>
       </c>
       <c r="H3">
         <v>21785</v>
@@ -926,7 +926,7 @@
         <v>89</v>
       </c>
       <c r="G4">
-        <v>20.8</v>
+        <v>21.3</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>141</v>
@@ -952,7 +952,7 @@
         <v>90</v>
       </c>
       <c r="G5">
-        <v>24.7</v>
+        <v>24.9</v>
       </c>
       <c r="H5">
         <v>25870</v>
@@ -978,7 +978,7 @@
         <v>89</v>
       </c>
       <c r="G6">
-        <v>18</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>141</v>
@@ -1004,7 +1004,7 @@
         <v>90</v>
       </c>
       <c r="G7">
-        <v>23.6</v>
+        <v>22.4</v>
       </c>
       <c r="H7">
         <v>22330</v>
@@ -1030,7 +1030,7 @@
         <v>89</v>
       </c>
       <c r="G8">
-        <v>18</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>141</v>
@@ -1082,7 +1082,7 @@
         <v>94</v>
       </c>
       <c r="G10">
-        <v>25.8</v>
+        <v>25.6</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>141</v>
@@ -1108,7 +1108,7 @@
         <v>90</v>
       </c>
       <c r="G11">
-        <v>27.9</v>
+        <v>28.1</v>
       </c>
       <c r="H11">
         <v>17870</v>
@@ -1134,7 +1134,7 @@
         <v>89</v>
       </c>
       <c r="G12">
-        <v>17.3</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>141</v>
@@ -1160,7 +1160,7 @@
         <v>90</v>
       </c>
       <c r="G13" s="2">
-        <v>21.5</v>
+        <v>22.2</v>
       </c>
       <c r="H13">
         <v>22890</v>
@@ -1186,7 +1186,7 @@
         <v>89</v>
       </c>
       <c r="G14">
-        <v>24.6</v>
+        <v>25.3</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>141</v>
@@ -1212,7 +1212,7 @@
         <v>90</v>
       </c>
       <c r="G15">
-        <v>30</v>
+        <v>29.5</v>
       </c>
       <c r="H15">
         <v>35875</v>
@@ -1238,7 +1238,7 @@
         <v>89</v>
       </c>
       <c r="G16">
-        <v>16.899999999999999</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>141</v>
@@ -1264,7 +1264,7 @@
         <v>90</v>
       </c>
       <c r="G17">
-        <v>20</v>
+        <v>20.9</v>
       </c>
       <c r="H17">
         <v>21607.5</v>
@@ -1290,7 +1290,7 @@
         <v>89</v>
       </c>
       <c r="G18">
-        <v>22.1</v>
+        <v>24.7</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>141</v>
@@ -1342,7 +1342,7 @@
         <v>89</v>
       </c>
       <c r="G20">
-        <v>25.6</v>
+        <v>27</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>141</v>
@@ -1368,7 +1368,7 @@
         <v>90</v>
       </c>
       <c r="G21">
-        <v>30.6</v>
+        <v>30.2</v>
       </c>
       <c r="H21">
         <v>22760</v>
@@ -1394,7 +1394,7 @@
         <v>91</v>
       </c>
       <c r="G22">
-        <v>24.1</v>
+        <v>26.5</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>141</v>
@@ -1420,7 +1420,7 @@
         <v>92</v>
       </c>
       <c r="G23">
-        <v>51.3</v>
+        <v>52.6</v>
       </c>
       <c r="H23">
         <v>54187.5</v>
@@ -1446,7 +1446,7 @@
         <v>91</v>
       </c>
       <c r="G24">
-        <v>17.5</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>141</v>
@@ -1472,7 +1472,7 @@
         <v>92</v>
       </c>
       <c r="G25">
-        <v>34.6</v>
+        <v>36.1</v>
       </c>
       <c r="H25">
         <v>40387.5</v>
@@ -1498,7 +1498,7 @@
         <v>91</v>
       </c>
       <c r="G26">
-        <v>23.2</v>
+        <v>23.9</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>141</v>
@@ -1524,7 +1524,7 @@
         <v>92</v>
       </c>
       <c r="G27">
-        <v>46.6</v>
+        <v>47.5</v>
       </c>
       <c r="H27">
         <v>38932.5</v>
@@ -1550,7 +1550,7 @@
         <v>91</v>
       </c>
       <c r="G28">
-        <v>24.8</v>
+        <v>26.9</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>141</v>
@@ -1576,7 +1576,7 @@
         <v>92</v>
       </c>
       <c r="G29">
-        <v>49.9</v>
+        <v>51.8</v>
       </c>
       <c r="H29">
         <v>57077.5</v>
@@ -1602,7 +1602,7 @@
         <v>91</v>
       </c>
       <c r="G30">
-        <v>19.600000000000001</v>
+        <v>21.1</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>141</v>
@@ -1628,7 +1628,7 @@
         <v>92</v>
       </c>
       <c r="G31">
-        <v>46.5</v>
+        <v>46.7</v>
       </c>
       <c r="H31">
         <v>37397.5</v>
@@ -1654,7 +1654,7 @@
         <v>91</v>
       </c>
       <c r="G32">
-        <v>16.600000000000001</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>141</v>
@@ -1680,7 +1680,7 @@
         <v>92</v>
       </c>
       <c r="G33">
-        <v>33.299999999999997</v>
+        <v>33.200000000000003</v>
       </c>
       <c r="H33">
         <v>37837.5</v>
@@ -1706,7 +1706,7 @@
         <v>91</v>
       </c>
       <c r="G34">
-        <v>18.100000000000001</v>
+        <v>18</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>141</v>
@@ -1732,7 +1732,7 @@
         <v>92</v>
       </c>
       <c r="G35">
-        <v>27.7</v>
+        <v>27.8</v>
       </c>
       <c r="H35">
         <v>28442.5</v>
@@ -1758,7 +1758,7 @@
         <v>92</v>
       </c>
       <c r="G36">
-        <v>42.1</v>
+        <v>41.9</v>
       </c>
       <c r="H36" s="2">
         <v>36430</v>
@@ -1784,7 +1784,7 @@
         <v>91</v>
       </c>
       <c r="G37">
-        <v>23.8</v>
+        <v>24.4</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>141</v>
@@ -1810,7 +1810,7 @@
         <v>92</v>
       </c>
       <c r="G38">
-        <v>53.4</v>
+        <v>53.5</v>
       </c>
       <c r="H38" s="2">
         <v>56740</v>
@@ -1836,7 +1836,7 @@
         <v>91</v>
       </c>
       <c r="G39">
-        <v>23.8</v>
+        <v>24.9</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>141</v>
@@ -1888,7 +1888,7 @@
         <v>93</v>
       </c>
       <c r="G41">
-        <v>26</v>
+        <v>23.2</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>141</v>
@@ -1914,7 +1914,7 @@
         <v>95</v>
       </c>
       <c r="G42">
-        <v>47.7</v>
+        <v>48.2</v>
       </c>
       <c r="H42">
         <v>45385</v>
@@ -1940,7 +1940,7 @@
         <v>93</v>
       </c>
       <c r="G43">
-        <v>23</v>
+        <v>23.8</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>141</v>
@@ -1966,7 +1966,7 @@
         <v>95</v>
       </c>
       <c r="G44">
-        <v>48.4</v>
+        <v>49.6</v>
       </c>
       <c r="H44">
         <v>39175</v>
@@ -1992,7 +1992,7 @@
         <v>93</v>
       </c>
       <c r="G45">
-        <v>25</v>
+        <v>25.3</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>141</v>
@@ -2070,7 +2070,7 @@
         <v>93</v>
       </c>
       <c r="G48">
-        <v>25.8</v>
+        <v>26.6</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>141</v>
@@ -2096,7 +2096,7 @@
         <v>95</v>
       </c>
       <c r="G49">
-        <v>49.8</v>
+        <v>50.5</v>
       </c>
       <c r="H49">
         <v>48600</v>
@@ -2122,7 +2122,7 @@
         <v>93</v>
       </c>
       <c r="G50">
-        <v>18.3</v>
+        <v>19.8</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>141</v>
@@ -2148,7 +2148,7 @@
         <v>95</v>
       </c>
       <c r="G51">
-        <v>48.4</v>
+        <v>45.9</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -2171,7 +2171,7 @@
         <v>93</v>
       </c>
       <c r="G52">
-        <v>17.600000000000001</v>
+        <v>17.7</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>141</v>
@@ -2197,7 +2197,7 @@
         <v>95</v>
       </c>
       <c r="G53">
-        <v>35.700000000000003</v>
+        <v>36.4</v>
       </c>
       <c r="H53">
         <v>32765</v>
@@ -2223,7 +2223,7 @@
         <v>93</v>
       </c>
       <c r="G54">
-        <v>16.399999999999999</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>141</v>
@@ -2249,7 +2249,7 @@
         <v>95</v>
       </c>
       <c r="G55">
-        <v>31.1</v>
+        <v>30.5</v>
       </c>
       <c r="H55">
         <v>32342.5</v>
@@ -2275,7 +2275,7 @@
         <v>93</v>
       </c>
       <c r="G56">
-        <v>18.100000000000001</v>
+        <v>18.2</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>141</v>
@@ -2301,7 +2301,7 @@
         <v>95</v>
       </c>
       <c r="G57">
-        <v>38.1</v>
+        <v>38.4</v>
       </c>
       <c r="H57">
         <v>24667.5</v>
@@ -2327,7 +2327,7 @@
         <v>93</v>
       </c>
       <c r="G58">
-        <v>20</v>
+        <v>20.3</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>141</v>
@@ -2353,7 +2353,7 @@
         <v>95</v>
       </c>
       <c r="G59">
-        <v>37</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="H59">
         <v>29167.5</v>
@@ -2379,7 +2379,7 @@
         <v>96</v>
       </c>
       <c r="G60">
-        <v>22.2</v>
+        <v>21.9</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>141</v>
@@ -2405,7 +2405,7 @@
         <v>97</v>
       </c>
       <c r="G61">
-        <v>47.8</v>
+        <v>48.8</v>
       </c>
       <c r="H61">
         <v>39510</v>
@@ -2431,7 +2431,7 @@
         <v>96</v>
       </c>
       <c r="G62">
-        <v>24</v>
+        <v>24.9</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>141</v>
@@ -2457,7 +2457,7 @@
         <v>96</v>
       </c>
       <c r="G63">
-        <v>23.5</v>
+        <v>24.5</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>141</v>
@@ -2483,7 +2483,7 @@
         <v>97</v>
       </c>
       <c r="G64">
-        <v>50.3</v>
+        <v>53.8</v>
       </c>
       <c r="H64" s="2">
         <v>47517.5</v>
@@ -2509,7 +2509,7 @@
         <v>96</v>
       </c>
       <c r="G65">
-        <v>25.9</v>
+        <v>26.4</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>141</v>
@@ -2535,7 +2535,7 @@
         <v>97</v>
       </c>
       <c r="G66">
-        <v>49.1</v>
+        <v>51.9</v>
       </c>
       <c r="H66">
         <v>58777.5</v>
@@ -2561,7 +2561,7 @@
         <v>96</v>
       </c>
       <c r="G67">
-        <v>17.3</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>141</v>
@@ -2587,7 +2587,7 @@
         <v>97</v>
       </c>
       <c r="G68">
-        <v>27.4</v>
+        <v>27.5</v>
       </c>
       <c r="H68">
         <v>30347.5</v>
@@ -2613,7 +2613,7 @@
         <v>96</v>
       </c>
       <c r="G69">
-        <v>18.5</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>141</v>
@@ -2639,7 +2639,7 @@
         <v>97</v>
       </c>
       <c r="G70">
-        <v>43.4</v>
+        <v>43.3</v>
       </c>
       <c r="H70">
         <v>39465</v>
@@ -2665,7 +2665,7 @@
         <v>96</v>
       </c>
       <c r="G71">
-        <v>25.4</v>
+        <v>25.7</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>141</v>
@@ -2691,7 +2691,7 @@
         <v>97</v>
       </c>
       <c r="G72">
-        <v>49.8</v>
+        <v>49.5</v>
       </c>
       <c r="H72">
         <v>50897.5</v>
@@ -2717,7 +2717,7 @@
         <v>96</v>
       </c>
       <c r="G73">
-        <v>19.7</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>141</v>
@@ -2743,7 +2743,7 @@
         <v>96</v>
       </c>
       <c r="G74">
-        <v>18.899999999999999</v>
+        <v>20.2</v>
       </c>
       <c r="H74" s="2" t="s">
         <v>141</v>
@@ -2769,7 +2769,7 @@
         <v>97</v>
       </c>
       <c r="G75">
-        <v>46.4</v>
+        <v>46.2</v>
       </c>
       <c r="H75">
         <v>35699.166669999999</v>
@@ -2795,7 +2795,7 @@
         <v>96</v>
       </c>
       <c r="G76">
-        <v>17</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>141</v>
@@ -2821,7 +2821,7 @@
         <v>97</v>
       </c>
       <c r="G77">
-        <v>35.299999999999997</v>
+        <v>34.4</v>
       </c>
       <c r="H77">
         <v>27257.5</v>

</xml_diff>

<commit_message>
Added SC6C blood glucose
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Stevia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EE241D-93BC-4E71-9028-A842EE49667C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802D1C9E-EF9D-415B-B7A9-0D19C4773C7A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{DE68B47F-C64E-46B0-840B-CBBCFE996E82}"/>
   </bookViews>
@@ -819,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F580D838-176B-498F-A508-C3968484E9F8}">
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2150,6 +2150,9 @@
       <c r="G51">
         <v>45.9</v>
       </c>
+      <c r="H51">
+        <v>32625</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">

</xml_diff>

<commit_message>
Updated metadata w/ Diet (Low vs. High Fat)
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Stevia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Li\Documents\Stevia\Stevia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802D1C9E-EF9D-415B-B7A9-0D19C4773C7A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA951D59-4AA4-49F2-8457-D22B1D39AB24}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{DE68B47F-C64E-46B0-840B-CBBCFE996E82}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="143">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -456,6 +456,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Diet</t>
   </si>
 </sst>
 </file>
@@ -817,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F580D838-176B-498F-A508-C3968484E9F8}">
-  <dimension ref="A1:H77"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M68" sqref="M68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -828,7 +831,7 @@
     <col min="1" max="5" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -848,13 +851,16 @@
         <v>88</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -873,14 +879,17 @@
       <c r="F2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2">
         <v>23.2</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -899,14 +908,17 @@
       <c r="F3" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3">
         <v>26.7</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>21785</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -925,14 +937,17 @@
       <c r="F4" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4">
         <v>21.3</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -951,14 +966,17 @@
       <c r="F5" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5">
         <v>24.9</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>25870</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -977,14 +995,17 @@
       <c r="F6" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6">
         <v>19.100000000000001</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1003,14 +1024,17 @@
       <c r="F7" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7">
         <v>22.4</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>22330</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1029,14 +1053,17 @@
       <c r="F8" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8">
         <v>18.600000000000001</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1055,14 +1082,17 @@
       <c r="F9" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9">
         <v>23</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>19890</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1081,14 +1111,17 @@
       <c r="F10" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10">
         <v>25.6</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1107,14 +1140,17 @@
       <c r="F11" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11">
         <v>28.1</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>17870</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1133,14 +1169,17 @@
       <c r="F12" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12">
         <v>18.600000000000001</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1159,14 +1198,17 @@
       <c r="F13" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H13" s="2">
         <v>22.2</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>22890</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1185,14 +1227,17 @@
       <c r="F14" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14">
         <v>25.3</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -1211,14 +1256,17 @@
       <c r="F15" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15">
         <v>29.5</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>35875</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -1237,14 +1285,17 @@
       <c r="F16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H16">
         <v>17.399999999999999</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1263,14 +1314,17 @@
       <c r="F17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17">
         <v>20.9</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>21607.5</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1289,14 +1343,17 @@
       <c r="F18" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H18">
         <v>24.7</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -1315,14 +1372,17 @@
       <c r="F19" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H19">
         <v>26.6</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>26352.5</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>5</v>
       </c>
@@ -1341,14 +1401,17 @@
       <c r="F20" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H20">
         <v>27</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>6</v>
       </c>
@@ -1367,14 +1430,17 @@
       <c r="F21" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H21">
         <v>30.2</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>22760</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
@@ -1393,14 +1459,17 @@
       <c r="F22" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H22">
         <v>26.5</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I22" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
@@ -1419,14 +1488,17 @@
       <c r="F23" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H23">
         <v>52.6</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>54187.5</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
@@ -1445,14 +1517,17 @@
       <c r="F24" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H24">
         <v>18.899999999999999</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I24" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
@@ -1471,14 +1546,17 @@
       <c r="F25" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H25">
         <v>36.1</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>40387.5</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
@@ -1497,14 +1575,17 @@
       <c r="F26" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26">
         <v>23.9</v>
       </c>
-      <c r="H26" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I26" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
@@ -1523,14 +1604,17 @@
       <c r="F27" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H27">
         <v>47.5</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>38932.5</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
@@ -1549,14 +1633,17 @@
       <c r="F28" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H28">
         <v>26.9</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I28" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
@@ -1575,14 +1662,17 @@
       <c r="F29" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H29">
         <v>51.8</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>57077.5</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>35</v>
       </c>
@@ -1601,14 +1691,17 @@
       <c r="F30" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H30">
         <v>21.1</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I30" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
@@ -1627,14 +1720,17 @@
       <c r="F31" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H31">
         <v>46.7</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>37397.5</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>37</v>
       </c>
@@ -1653,14 +1749,17 @@
       <c r="F32" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H32">
         <v>18.100000000000001</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I32" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>38</v>
       </c>
@@ -1679,14 +1778,17 @@
       <c r="F33" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H33">
         <v>33.200000000000003</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>37837.5</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
@@ -1705,14 +1807,17 @@
       <c r="F34" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H34">
         <v>18</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I34" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>40</v>
       </c>
@@ -1731,14 +1836,17 @@
       <c r="F35" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H35">
         <v>27.8</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <v>28442.5</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
@@ -1757,14 +1865,17 @@
       <c r="F36" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H36">
         <v>41.9</v>
       </c>
-      <c r="H36" s="2">
+      <c r="I36" s="2">
         <v>36430</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>42</v>
       </c>
@@ -1783,14 +1894,17 @@
       <c r="F37" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H37">
         <v>24.4</v>
       </c>
-      <c r="H37" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I37" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
@@ -1809,14 +1923,17 @@
       <c r="F38" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H38">
         <v>53.5</v>
       </c>
-      <c r="H38" s="2">
+      <c r="I38" s="2">
         <v>56740</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>25</v>
       </c>
@@ -1835,14 +1952,17 @@
       <c r="F39" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H39">
         <v>24.9</v>
       </c>
-      <c r="H39" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I39" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>26</v>
       </c>
@@ -1861,14 +1981,17 @@
       <c r="F40" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H40">
         <v>48.7</v>
       </c>
-      <c r="H40" s="2">
+      <c r="I40" s="2">
         <v>29777.5</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>46</v>
       </c>
@@ -1887,14 +2010,17 @@
       <c r="F41" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H41">
         <v>23.2</v>
       </c>
-      <c r="H41" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I41" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>47</v>
       </c>
@@ -1913,14 +2039,17 @@
       <c r="F42" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H42">
         <v>48.2</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <v>45385</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>48</v>
       </c>
@@ -1939,14 +2068,17 @@
       <c r="F43" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H43">
         <v>23.8</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I43" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>49</v>
       </c>
@@ -1965,14 +2097,17 @@
       <c r="F44" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H44">
         <v>49.6</v>
       </c>
-      <c r="H44">
+      <c r="I44">
         <v>39175</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>50</v>
       </c>
@@ -1991,14 +2126,17 @@
       <c r="F45" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H45">
         <v>25.3</v>
       </c>
-      <c r="H45" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I45" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
@@ -2017,14 +2155,17 @@
       <c r="F46" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H46">
         <v>48.1</v>
       </c>
-      <c r="H46">
+      <c r="I46">
         <v>48645.833299999998</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>52</v>
       </c>
@@ -2043,14 +2184,17 @@
       <c r="F47" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H47">
         <v>22.2</v>
       </c>
-      <c r="H47" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I47" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>53</v>
       </c>
@@ -2069,14 +2213,17 @@
       <c r="F48" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H48">
         <v>26.6</v>
       </c>
-      <c r="H48" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I48" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>54</v>
       </c>
@@ -2095,14 +2242,17 @@
       <c r="F49" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H49">
         <v>50.5</v>
       </c>
-      <c r="H49">
+      <c r="I49">
         <v>48600</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>55</v>
       </c>
@@ -2121,14 +2271,17 @@
       <c r="F50" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H50">
         <v>19.8</v>
       </c>
-      <c r="H50" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I50" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>56</v>
       </c>
@@ -2147,14 +2300,17 @@
       <c r="F51" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H51">
         <v>45.9</v>
       </c>
-      <c r="H51">
+      <c r="I51">
         <v>32625</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>57</v>
       </c>
@@ -2173,14 +2329,17 @@
       <c r="F52" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H52">
         <v>17.7</v>
       </c>
-      <c r="H52" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I52" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>58</v>
       </c>
@@ -2199,14 +2358,17 @@
       <c r="F53" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H53">
         <v>36.4</v>
       </c>
-      <c r="H53">
+      <c r="I53">
         <v>32765</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
@@ -2225,14 +2387,17 @@
       <c r="F54" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H54">
         <v>17.600000000000001</v>
       </c>
-      <c r="H54" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I54" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>60</v>
       </c>
@@ -2251,14 +2416,17 @@
       <c r="F55" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G55">
+      <c r="G55" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H55">
         <v>30.5</v>
       </c>
-      <c r="H55">
+      <c r="I55">
         <v>32342.5</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>61</v>
       </c>
@@ -2277,14 +2445,17 @@
       <c r="F56" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H56">
         <v>18.2</v>
       </c>
-      <c r="H56" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I56" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>62</v>
       </c>
@@ -2303,14 +2474,17 @@
       <c r="F57" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H57">
         <v>38.4</v>
       </c>
-      <c r="H57">
+      <c r="I57">
         <v>24667.5</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>44</v>
       </c>
@@ -2329,14 +2503,17 @@
       <c r="F58" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G58">
+      <c r="G58" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H58">
         <v>20.3</v>
       </c>
-      <c r="H58" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I58" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>45</v>
       </c>
@@ -2355,14 +2532,17 @@
       <c r="F59" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H59">
         <v>36.700000000000003</v>
       </c>
-      <c r="H59">
+      <c r="I59">
         <v>29167.5</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>65</v>
       </c>
@@ -2381,14 +2561,17 @@
       <c r="F60" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G60">
+      <c r="G60" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H60">
         <v>21.9</v>
       </c>
-      <c r="H60" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I60" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>66</v>
       </c>
@@ -2407,14 +2590,17 @@
       <c r="F61" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H61">
         <v>48.8</v>
       </c>
-      <c r="H61">
+      <c r="I61">
         <v>39510</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>67</v>
       </c>
@@ -2433,14 +2619,17 @@
       <c r="F62" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G62">
+      <c r="G62" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H62">
         <v>24.9</v>
       </c>
-      <c r="H62" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I62" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>68</v>
       </c>
@@ -2459,14 +2648,17 @@
       <c r="F63" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G63">
+      <c r="G63" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H63">
         <v>24.5</v>
       </c>
-      <c r="H63" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I63" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>69</v>
       </c>
@@ -2485,14 +2677,17 @@
       <c r="F64" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G64">
+      <c r="G64" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H64">
         <v>53.8</v>
       </c>
-      <c r="H64" s="2">
+      <c r="I64" s="2">
         <v>47517.5</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>70</v>
       </c>
@@ -2511,14 +2706,17 @@
       <c r="F65" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G65">
+      <c r="G65" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H65">
         <v>26.4</v>
       </c>
-      <c r="H65" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I65" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>71</v>
       </c>
@@ -2537,14 +2735,17 @@
       <c r="F66" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G66">
+      <c r="G66" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H66">
         <v>51.9</v>
       </c>
-      <c r="H66">
+      <c r="I66">
         <v>58777.5</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>72</v>
       </c>
@@ -2563,14 +2764,17 @@
       <c r="F67" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G67">
+      <c r="G67" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H67">
         <v>17.100000000000001</v>
       </c>
-      <c r="H67" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I67" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>73</v>
       </c>
@@ -2589,14 +2793,17 @@
       <c r="F68" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G68">
+      <c r="G68" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H68">
         <v>27.5</v>
       </c>
-      <c r="H68">
+      <c r="I68">
         <v>30347.5</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>74</v>
       </c>
@@ -2615,14 +2822,17 @@
       <c r="F69" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G69">
+      <c r="G69" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H69">
         <v>18.100000000000001</v>
       </c>
-      <c r="H69" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I69" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>75</v>
       </c>
@@ -2641,14 +2851,17 @@
       <c r="F70" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G70">
+      <c r="G70" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H70">
         <v>43.3</v>
       </c>
-      <c r="H70">
+      <c r="I70">
         <v>39465</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>76</v>
       </c>
@@ -2667,14 +2880,17 @@
       <c r="F71" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G71">
+      <c r="G71" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H71">
         <v>25.7</v>
       </c>
-      <c r="H71" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I71" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>77</v>
       </c>
@@ -2693,14 +2909,17 @@
       <c r="F72" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G72">
+      <c r="G72" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H72">
         <v>49.5</v>
       </c>
-      <c r="H72">
+      <c r="I72">
         <v>50897.5</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>98</v>
       </c>
@@ -2719,14 +2938,17 @@
       <c r="F73" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G73">
+      <c r="G73" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H73">
         <v>19.399999999999999</v>
       </c>
-      <c r="H73" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I73" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>78</v>
       </c>
@@ -2745,14 +2967,17 @@
       <c r="F74" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G74">
+      <c r="G74" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H74">
         <v>20.2</v>
       </c>
-      <c r="H74" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I74" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>79</v>
       </c>
@@ -2771,14 +2996,17 @@
       <c r="F75" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G75">
+      <c r="G75" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H75">
         <v>46.2</v>
       </c>
-      <c r="H75">
+      <c r="I75">
         <v>35699.166669999999</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>63</v>
       </c>
@@ -2797,14 +3025,17 @@
       <c r="F76" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G76">
+      <c r="G76" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H76">
         <v>19.100000000000001</v>
       </c>
-      <c r="H76" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I76" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>64</v>
       </c>
@@ -2823,10 +3054,13 @@
       <c r="F77" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G77">
+      <c r="G77" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H77">
         <v>34.4</v>
       </c>
-      <c r="H77">
+      <c r="I77">
         <v>27257.5</v>
       </c>
     </row>

</xml_diff>